<commit_message>
Updated with quarterly data.
</commit_message>
<xml_diff>
--- a/PL/PL.xlsx
+++ b/PL/PL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/534a1defcf7f9d1a/Company Models CloudSave/PL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="968" documentId="8_{DD1FE8FB-81A2-451C-9233-98A045FFB118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F13B205A-12ED-43A6-A546-B1FA6DF9C58B}"/>
+  <xr:revisionPtr revIDLastSave="977" documentId="8_{DD1FE8FB-81A2-451C-9233-98A045FFB118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60DDCF89-2AC5-4C76-B02D-C20F3FCA2FFC}"/>
   <bookViews>
-    <workbookView xWindow="39970" yWindow="3050" windowWidth="26720" windowHeight="17120" activeTab="2" xr2:uid="{F70D17C0-3989-48E5-BF07-6389F34DDC43}"/>
+    <workbookView minimized="1" xWindow="9060" yWindow="2740" windowWidth="26720" windowHeight="17120" activeTab="2" xr2:uid="{F70D17C0-3989-48E5-BF07-6389F34DDC43}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -818,8 +818,8 @@
     <v>6.27</v>
     <v>2.46</v>
     <v>1.496</v>
-    <v>-0.03</v>
-    <v>-1.1672999999999999E-2</v>
+    <v>0.05</v>
+    <v>1.9762999999999999E-2</v>
     <v>USD</v>
     <v>Planet Labs PBC is a provider of global, daily satellite imagery and geospatial solutions. The Company designs, builds, and operates the earth observation fleet of imaging satellites, capturing, and compiling data. Its satellite data and analytics reveal actionable insights regarding a large array of important phenomena, such as deforestation, agriculture, climate change, biodiversity, and supply chains worldwide. Its daily stream of proprietary data and machine learning analytics, delivered over its cloud-native platform, helps companies, governments, and civil society use satellite imagery to discover insights as change happens. It serves approximately 880 customers across large commercial and government verticals, including agriculture, mapping, forestry, finance, and insurance, as well as federal, state, and local government bodies. It also owns Sentinel Hub, an advanced API-driven, cloud streaming platform that allows customers to access multi-source earth observation (EO) data.</v>
     <v>930</v>
@@ -827,23 +827,23 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>645 Harrison Street, Floor 4, SAN FRANCISCO, CA, 94107 US</v>
-    <v>2.57</v>
+    <v>2.61</v>
     <v>Aerospace &amp; Defense</v>
     <v>Stock</v>
-    <v>45202.653726897654</v>
+    <v>45203.755070207815</v>
     <v>0</v>
-    <v>2.5249999999999999</v>
-    <v>725575892</v>
+    <v>2.5</v>
+    <v>737002284</v>
     <v>PLANET LABS PBC</v>
     <v>PLANET LABS PBC</v>
-    <v>2.5649999999999999</v>
-    <v>2.57</v>
     <v>2.54</v>
+    <v>2.5299999999999998</v>
+    <v>2.58</v>
     <v>285659800</v>
     <v>PL</v>
     <v>PLANET LABS PBC (XNYS:PL)</v>
-    <v>305469</v>
-    <v>1799582</v>
+    <v>636320</v>
+    <v>1790837</v>
     <v>2020</v>
   </rv>
   <rv s="2">
@@ -1425,7 +1425,7 @@
       </c>
       <c r="B2" s="2" cm="1">
         <f t="array" ref="B2">_FV(A1,"Price")</f>
-        <v>2.54</v>
+        <v>2.58</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1446,7 +1446,7 @@
       </c>
       <c r="B4" s="2">
         <f>B2*B3</f>
-        <v>725.57589200000007</v>
+        <v>737.00228400000003</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -1619,10 +1619,10 @@
   <dimension ref="B1:AH120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="H134" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="7" topLeftCell="H17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="R92" sqref="R92"/>
+      <selection pane="bottomRight" activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>